<commit_message>
made class and methods and interface, mostly done
</commit_message>
<xml_diff>
--- a/parts_list.xlsx
+++ b/parts_list.xlsx
@@ -1,50 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\Desktop\Project R33 Thangs\Godzillas-Parts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8C09B-EB07-448C-91FB-17F7A2DD1EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12552" windowWidth="23232" xWindow="-96" yWindow="-96"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Total Parts List</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Purchase Price</t>
+  </si>
+  <si>
+    <t>Total Spent</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,18 +101,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -377,79 +421,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col customWidth="1" max="2" min="2" width="13.3671875"/>
-    <col customWidth="1" max="3" min="3" width="14.3125"/>
-    <col customWidth="1" max="4" min="4" width="19.7890625"/>
-    <col customWidth="1" max="6" min="6" width="12.15625"/>
+    <col min="2" max="2" width="13.3671875" customWidth="1"/>
+    <col min="3" max="3" width="14.3125" customWidth="1"/>
+    <col min="4" max="4" width="19.7890625" customWidth="1"/>
+    <col min="6" max="6" width="12.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Total Parts List</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>Brand</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Part</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>Purchase Price</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>Total Spent</t>
-        </is>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F5" s="2">
         <f>SUM(D6:D2000)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Nismo</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Fuel Pump</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>